<commit_message>
modified excel comments & casing in comments
</commit_message>
<xml_diff>
--- a/spec_files/Specified_Lines.xlsx
+++ b/spec_files/Specified_Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\utility\nemo_in_action\spec_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8F1822-FA0D-48D6-BEFA-30D8CB37F693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E22068-3358-4542-A52B-50F4F1343ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{DFA622AB-CF54-4338-890D-DE7B128FB835}"/>
   </bookViews>
@@ -66,17 +66,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>John:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Episode Name / File Name</t>
+          <t>File Name</t>
         </r>
       </text>
     </comment>
@@ -90,17 +80,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>John:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>Line to search for</t>
         </r>
       </text>
     </comment>

</xml_diff>